<commit_message>
README updated with executive summary and data information section. Docs folder added for github pages.
</commit_message>
<xml_diff>
--- a/Excel/under65_stroke_risk_project_v6.xlsx
+++ b/Excel/under65_stroke_risk_project_v6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarpy\Documents\portfolio_projects\under_65_stroke_risk\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF549E7F-0F25-4C93-9205-A5B7DD8D3285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F507939-0814-425A-BB98-7080FB629B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="9" activeTab="9" xr2:uid="{D13153F3-D28B-4BE2-A42F-38EF5B75FFD3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="5" xr2:uid="{D13153F3-D28B-4BE2-A42F-38EF5B75FFD3}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -5015,7 +5015,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5031,6 +5031,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5119,7 +5125,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5411,6 +5417,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -54882,7 +54900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6126C36F-F768-4888-8727-5FE45433CBEE}">
   <dimension ref="B2:M142"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A109" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A109" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="L132" sqref="L132"/>
     </sheetView>
   </sheetViews>
@@ -58604,7 +58622,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" ht="41.4" x14ac:dyDescent="0.3">
       <c r="B26" s="47">
         <v>24</v>
       </c>
@@ -59179,10 +59197,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C8A1403-F8AB-46A4-B7AB-76C505A072E0}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -59197,159 +59218,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="107" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="107" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="104">
         <v>45820</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="104">
         <v>45821</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="4" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="104">
         <v>45821</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="104">
         <v>45821</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="4" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="104">
         <v>45821</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="4" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="104">
         <v>45821</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="5" t="s">
         <v>83</v>
       </c>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="104">
         <v>45821</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="4" t="s">
         <v>129</v>
       </c>
     </row>
@@ -59365,7 +59387,8 @@
       <formula>"not started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="68" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
README update, work done from executive summary to age vs feature. Visuals modified and copied from presentation slides using a copy.
</commit_message>
<xml_diff>
--- a/Excel/under65_stroke_risk_project_v6.xlsx
+++ b/Excel/under65_stroke_risk_project_v6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarpy\Documents\portfolio_projects\under_65_stroke_risk\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F507939-0814-425A-BB98-7080FB629B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9CFC18-3264-47A5-8AF5-4494DD36D817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="5" xr2:uid="{D13153F3-D28B-4BE2-A42F-38EF5B75FFD3}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="9" activeTab="3" xr2:uid="{D13153F3-D28B-4BE2-A42F-38EF5B75FFD3}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -1948,161 +1948,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1. Never smoked and unknown status patients represent roughly </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>69%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of the data.
-2. Having a history of smoking (smokes, formerly smokes) showed a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>higher stroke rate</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(3.79% </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3.76%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">).
-3. Smoking or formerly smoked shows </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>almost double</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the rate of stroke occurence compared to the other groups.
-4. Smokes and formerly smokes contributed roughly the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>same number of stroke occurences</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> while being roughly </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>half the size</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of the other two groups.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>1. Patients within the normal and overweight categories make up</t>
     </r>
     <r>
@@ -2671,139 +2516,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> stroke rate among patients without hypertension. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. The </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Chi-Square Test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is was used to evaluate the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>statistical significance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of categorical features in relation to the target variabel (stroke).
-2. Both</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> gender and residence_type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> had p-values that were </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">greater than the 0.05 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">significance threshold, indicating </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>no statistical significant association</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> between these two features and stroke in patients under 65.
-3. As a result, gender and residence type will be </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>excluded from further analysis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
     </r>
   </si>
   <si>
@@ -3646,14 +3358,6 @@
   </si>
   <si>
     <t>Bin Continuous Features</t>
-  </si>
-  <si>
-    <t>Based on CDC Standards, the age group was binned into:
-* children(0-17), youngadult(18-24),  adults(25-34), midlife adults(34-44), older adults(45-54), pre-seniors(55-64)
-Bsed on CDC standards, avg_glucose_level was binned into:
-* hypoglycemic(&lt;70), normal (70-99), pre-diabetic (100-125), diabetic (126-199), and high diabetes (200+)
-Based on CDC standards, bmi was binned into:
-* underweight, normal weight, overweight, obesity class 1, obsesity class 2, and obesity class 3</t>
   </si>
   <si>
     <t>Under 65</t>
@@ -4822,6 +4526,302 @@
 4) A recruiter-facing README summary to showcase analysis process and results.</t>
     </r>
   </si>
+  <si>
+    <t>Based on CDC Standards, the age group was binned into:
+* children(0-17), young adult(18-24),  adults(25-34), midlife adults(34-44), older adults(45-54), pre-seniors(55-64)
+Based on CDC standards, avg_glucose_level was binned into:
+* hypoglycemic(&lt;70), normal (70-99), pre-diabetic (100-125), diabetic (126-199), and high diabetes (200+)
+Based on CDC standards, bmi was binned into:
+* underweight, normal weight, overweight, obesity class 1, obesity class 2, and obesity class 3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Never smoked and unknown status patients represent roughly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>69%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the data.
+2. Having a history of smoking (smokes, formerly smokes) showed a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>higher stroke rate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(3.79% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.76%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">).
+3. Smoking or formerly smoked shows </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>almost double</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the rate of stroke occurrence compared to the other groups.
+4. Smokes and formerly smokes contributed roughly the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>same number of stroke occurrences</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> while being roughly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>half the size</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the other two groups.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chi-Square Test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is was used to evaluate the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>statistical significance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of categorical features in relation to the target variable (stroke).
+2. Both</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> gender and residence_type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> had p-values that were </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">greater than the 0.05 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">significance threshold, indicating </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>no statistical significant association</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> between these two features and stroke in patients under 65.
+3. As a result, gender and residence type will be </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>excluded from further analysis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -5363,6 +5363,18 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5417,18 +5429,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -54483,32 +54483,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
-        <v>325</v>
-      </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
+      <c r="A1" s="89" t="s">
+        <v>322</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
     </row>
     <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="86"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
+      <c r="A2" s="90"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
       <c r="M2" s="7" t="s">
         <v>7</v>
       </c>
@@ -54520,17 +54520,17 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="86"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
+      <c r="A3" s="90"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
       <c r="M3" s="3" t="s">
         <v>0</v>
       </c>
@@ -54542,17 +54542,17 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="86"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
+      <c r="A4" s="90"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
       <c r="M4" s="3" t="s">
         <v>3</v>
       </c>
@@ -54564,17 +54564,17 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="86"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
+      <c r="A5" s="90"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
       <c r="M5" s="3" t="s">
         <v>5</v>
       </c>
@@ -54586,17 +54586,17 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="86"/>
-      <c r="B6" s="86"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="86"/>
+      <c r="A6" s="90"/>
+      <c r="B6" s="90"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
       <c r="M6" s="3" t="s">
         <v>15</v>
       </c>
@@ -54608,17 +54608,17 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="86"/>
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
+      <c r="A7" s="90"/>
+      <c r="B7" s="90"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="90"/>
+      <c r="E7" s="90"/>
+      <c r="F7" s="90"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="90"/>
       <c r="M7" s="3" t="s">
         <v>16</v>
       </c>
@@ -54630,17 +54630,17 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="86"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="86"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="86"/>
+      <c r="A8" s="90"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
       <c r="M8" s="3" t="s">
         <v>10</v>
       </c>
@@ -54652,17 +54652,17 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="86"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
+      <c r="A9" s="90"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="90"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
       <c r="M9" s="3" t="s">
         <v>13</v>
       </c>
@@ -54674,218 +54674,218 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="86"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
+      <c r="A10" s="90"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="90"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="86"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
+      <c r="A11" s="90"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="90"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="86"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
+      <c r="A12" s="90"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
       <c r="M12"/>
       <c r="N12"/>
       <c r="O12"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="86"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
+      <c r="A13" s="90"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="86"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
+      <c r="A14" s="90"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="90"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="86"/>
-      <c r="B15" s="86"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86"/>
-      <c r="K15" s="86"/>
+      <c r="A15" s="90"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="90"/>
+      <c r="J15" s="90"/>
+      <c r="K15" s="90"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="86"/>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="86"/>
-      <c r="K16" s="86"/>
+      <c r="A16" s="90"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="90"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="86"/>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="86"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="86"/>
-      <c r="K17" s="86"/>
+      <c r="A17" s="90"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="90"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="86"/>
-      <c r="B18" s="86"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="86"/>
+      <c r="A18" s="90"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="86"/>
-      <c r="B19" s="86"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
-      <c r="H19" s="86"/>
-      <c r="I19" s="86"/>
-      <c r="J19" s="86"/>
-      <c r="K19" s="86"/>
+      <c r="A19" s="90"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="90"/>
+      <c r="K19" s="90"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="86"/>
-      <c r="B20" s="86"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
-      <c r="H20" s="86"/>
-      <c r="I20" s="86"/>
-      <c r="J20" s="86"/>
-      <c r="K20" s="86"/>
+      <c r="A20" s="90"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="90"/>
+      <c r="K20" s="90"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="86"/>
-      <c r="B21" s="86"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="86"/>
-      <c r="J21" s="86"/>
-      <c r="K21" s="86"/>
+      <c r="A21" s="90"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="90"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="90"/>
+      <c r="K21" s="90"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="86"/>
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86"/>
-      <c r="H22" s="86"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="86"/>
-      <c r="K22" s="86"/>
+      <c r="A22" s="90"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="90"/>
+      <c r="H22" s="90"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="90"/>
+      <c r="K22" s="90"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="86"/>
-      <c r="B23" s="86"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="86"/>
-      <c r="J23" s="86"/>
-      <c r="K23" s="86"/>
+      <c r="A23" s="90"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="90"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="90"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="86"/>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86"/>
-      <c r="H24" s="86"/>
-      <c r="I24" s="86"/>
-      <c r="J24" s="86"/>
-      <c r="K24" s="86"/>
+      <c r="A24" s="90"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="90"/>
+      <c r="G24" s="90"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
+      <c r="J24" s="90"/>
+      <c r="K24" s="90"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="86"/>
-      <c r="B25" s="86"/>
-      <c r="C25" s="86"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
-      <c r="H25" s="86"/>
-      <c r="I25" s="86"/>
-      <c r="J25" s="86"/>
-      <c r="K25" s="86"/>
+      <c r="A25" s="90"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
+      <c r="G25" s="90"/>
+      <c r="H25" s="90"/>
+      <c r="I25" s="90"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -55743,12 +55743,12 @@
       <c r="I77" s="53"/>
     </row>
     <row r="96" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B96" s="98" t="s">
-        <v>289</v>
-      </c>
-      <c r="C96" s="98"/>
-      <c r="D96" s="98"/>
-      <c r="E96" s="98"/>
+      <c r="B96" s="102" t="s">
+        <v>286</v>
+      </c>
+      <c r="C96" s="102"/>
+      <c r="D96" s="102"/>
+      <c r="E96" s="102"/>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B97" s="59" t="s">
@@ -55828,7 +55828,7 @@
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C102" s="18">
         <v>0.15874571288584027</v>
@@ -55856,7 +55856,7 @@
     </row>
     <row r="104" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C104" s="80">
         <v>0.30475257226849584</v>
@@ -56471,12 +56471,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="98" t="s">
+      <c r="B2" s="102" t="s">
         <v>237</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="59" t="s">
@@ -56489,7 +56489,7 @@
         <v>228</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
@@ -56581,12 +56581,12 @@
       </c>
     </row>
     <row r="27" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B27" s="98" t="s">
+      <c r="B27" s="102" t="s">
         <v>239</v>
       </c>
-      <c r="C27" s="98"/>
-      <c r="D27" s="98"/>
-      <c r="E27" s="98"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="102"/>
+      <c r="E27" s="102"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="59" t="s">
@@ -56599,7 +56599,7 @@
         <v>229</v>
       </c>
       <c r="E28" s="59" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
@@ -56613,7 +56613,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="18" x14ac:dyDescent="0.35">
@@ -56692,12 +56692,12 @@
       </c>
     </row>
     <row r="52" spans="2:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="B52" s="98" t="s">
-        <v>280</v>
-      </c>
-      <c r="C52" s="98"/>
-      <c r="D52" s="98"/>
-      <c r="E52" s="98"/>
+      <c r="B52" s="102" t="s">
+        <v>277</v>
+      </c>
+      <c r="C52" s="102"/>
+      <c r="D52" s="102"/>
+      <c r="E52" s="102"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="59" t="s">
@@ -56710,7 +56710,7 @@
         <v>231</v>
       </c>
       <c r="E53" s="59" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
@@ -56724,7 +56724,7 @@
         <v>0.1028</v>
       </c>
       <c r="E54" s="61" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.3">
@@ -56964,21 +56964,21 @@
       </c>
     </row>
     <row r="103" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B103" s="103" t="s">
-        <v>282</v>
-      </c>
-      <c r="C103" s="103"/>
-      <c r="D103" s="103"/>
+      <c r="B103" s="107" t="s">
+        <v>279</v>
+      </c>
+      <c r="C103" s="107"/>
+      <c r="D103" s="107"/>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B104" s="76" t="s">
         <v>230</v>
       </c>
       <c r="C104" s="77" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D104" s="76" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.3">
@@ -56989,7 +56989,7 @@
         <v>3.9699999999999999E-2</v>
       </c>
       <c r="D105" s="72" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.3">
@@ -57173,13 +57173,13 @@
   <sheetData>
     <row r="2" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="83" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C2" s="83" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="84" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
@@ -57187,7 +57187,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
@@ -57195,10 +57195,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -57206,10 +57206,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -57217,10 +57217,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="100.8" x14ac:dyDescent="0.3">
@@ -57228,10 +57228,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -57239,10 +57239,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -57250,10 +57250,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -57261,10 +57261,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -57272,10 +57272,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -57283,10 +57283,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -57294,10 +57294,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -57305,10 +57305,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -57316,10 +57316,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="72" x14ac:dyDescent="0.3">
@@ -57327,10 +57327,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -57338,10 +57338,10 @@
         <v>15</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -57349,10 +57349,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -57360,10 +57360,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -57371,10 +57371,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -58239,14 +58239,14 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="87" t="s">
+      <c r="B15" s="91" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="87"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -58264,8 +58264,8 @@
   </sheetPr>
   <dimension ref="B1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -58279,12 +58279,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="92" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="44" t="s">
@@ -58378,10 +58378,10 @@
         <v>45821</v>
       </c>
       <c r="D8" s="50" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>269</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="55.2" x14ac:dyDescent="0.3">
@@ -58479,7 +58479,7 @@
         <v>173</v>
       </c>
       <c r="E15" s="51" t="s">
-        <v>252</v>
+        <v>324</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="69" x14ac:dyDescent="0.3">
@@ -58493,7 +58493,7 @@
         <v>185</v>
       </c>
       <c r="E16" s="49" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="88.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -58507,7 +58507,7 @@
         <v>198</v>
       </c>
       <c r="E17" s="51" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="55.2" x14ac:dyDescent="0.3">
@@ -58521,7 +58521,7 @@
         <v>197</v>
       </c>
       <c r="E18" s="49" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="55.2" x14ac:dyDescent="0.3">
@@ -58535,7 +58535,7 @@
         <v>202</v>
       </c>
       <c r="E19" s="49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="69" x14ac:dyDescent="0.3">
@@ -58549,7 +58549,7 @@
         <v>214</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>257</v>
+        <v>325</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="41.4" x14ac:dyDescent="0.3">
@@ -58563,7 +58563,7 @@
         <v>218</v>
       </c>
       <c r="E21" s="49" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="82.8" x14ac:dyDescent="0.3">
@@ -58577,7 +58577,7 @@
         <v>226</v>
       </c>
       <c r="E22" s="49" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="27.6" x14ac:dyDescent="0.3">
@@ -58591,7 +58591,7 @@
         <v>224</v>
       </c>
       <c r="E23" s="49" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -58605,7 +58605,7 @@
         <v>225</v>
       </c>
       <c r="E24" s="51" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="41.4" x14ac:dyDescent="0.3">
@@ -58619,7 +58619,7 @@
         <v>238</v>
       </c>
       <c r="E25" s="49" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="41.4" x14ac:dyDescent="0.3">
@@ -58633,7 +58633,7 @@
         <v>240</v>
       </c>
       <c r="E26" s="49" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="55.2" x14ac:dyDescent="0.3">
@@ -58647,7 +58647,7 @@
         <v>241</v>
       </c>
       <c r="E27" s="49" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="55.2" x14ac:dyDescent="0.3">
@@ -58661,15 +58661,15 @@
         <v>242</v>
       </c>
       <c r="E28" s="49" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="59" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="87" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -58677,7 +58677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A67A04FD-F1F5-41CF-A85B-7876F5D9F697}">
   <dimension ref="B2:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -58723,10 +58723,10 @@
         <v>94</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
@@ -58767,131 +58767,131 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="94" t="s">
         <v>176</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="90"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
-      <c r="I6" s="90"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="90"/>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="90"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="90"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="90"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="90"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="94"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="94"/>
+      <c r="I10" s="94"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="90"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="90"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="90"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="94"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="94"/>
+      <c r="I12" s="94"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="90"/>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="94"/>
+      <c r="I13" s="94"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="90"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="94"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="90"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="94"/>
+      <c r="I15" s="94"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>222</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C18" s="2">
         <v>90</v>
@@ -58903,7 +58903,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C19" s="2">
         <v>159</v>
@@ -58933,13 +58933,13 @@
         <v>133</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E34"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="6" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C35" s="6">
         <v>4082</v>
@@ -58950,7 +58950,7 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="6" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C36" s="6">
         <v>1027</v>
@@ -59095,7 +59095,7 @@
         <v>110</v>
       </c>
       <c r="M4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
@@ -59136,7 +59136,7 @@
         <v>110</v>
       </c>
       <c r="M5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
@@ -59177,7 +59177,7 @@
         <v>110</v>
       </c>
       <c r="M6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
@@ -59202,7 +59202,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -59218,22 +59218,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="105" t="s">
+      <c r="C1" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="107" t="s">
+      <c r="D1" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="105" t="s">
+      <c r="E1" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="107" t="s">
+      <c r="F1" s="88" t="s">
         <v>79</v>
       </c>
     </row>
@@ -59241,7 +59241,7 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="104">
+      <c r="B2" s="85">
         <v>45820</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -59261,7 +59261,7 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="104">
+      <c r="B3" s="85">
         <v>45821</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -59281,7 +59281,7 @@
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="104">
+      <c r="B4" s="85">
         <v>45821</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -59301,7 +59301,7 @@
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="104">
+      <c r="B5" s="85">
         <v>45821</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -59321,7 +59321,7 @@
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="104">
+      <c r="B6" s="85">
         <v>45821</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -59341,7 +59341,7 @@
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="104">
+      <c r="B7" s="85">
         <v>45821</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -59359,7 +59359,7 @@
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="104">
+      <c r="B8" s="85">
         <v>45821</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -59415,14 +59415,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="95" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
     </row>
     <row r="3" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
@@ -59565,16 +59565,16 @@
       </c>
     </row>
     <row r="27" spans="2:24" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B27" s="91" t="s">
+      <c r="B27" s="95" t="s">
         <v>192</v>
       </c>
-      <c r="C27" s="91"/>
-      <c r="D27" s="91"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="91"/>
-      <c r="G27" s="91"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="95"/>
       <c r="U27" s="78" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="V27" s="79" t="s">
         <v>137</v>
@@ -59606,7 +59606,7 @@
         <v>138</v>
       </c>
       <c r="U28" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="V28" s="18">
         <f>X28/W28</f>
@@ -59639,7 +59639,7 @@
         <v>0.1</v>
       </c>
       <c r="U29" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="V29" s="18">
         <f>X29/W29</f>
@@ -59691,8 +59691,8 @@
       <c r="G31" s="19">
         <v>0.18890000000000001</v>
       </c>
-      <c r="I31" s="94"/>
-      <c r="J31" s="94"/>
+      <c r="I31" s="98"/>
+      <c r="J31" s="98"/>
       <c r="V31" s="60">
         <f>V29/V28</f>
         <v>2.7844214270767944</v>
@@ -59717,8 +59717,8 @@
       <c r="G32" s="19">
         <v>0.15559999999999999</v>
       </c>
-      <c r="I32" s="94"/>
-      <c r="J32" s="94"/>
+      <c r="I32" s="98"/>
+      <c r="J32" s="98"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
@@ -59739,18 +59739,18 @@
       <c r="G33" s="19">
         <v>0.18890000000000001</v>
       </c>
-      <c r="I33" s="94"/>
-      <c r="J33" s="94"/>
+      <c r="I33" s="98"/>
+      <c r="J33" s="98"/>
     </row>
     <row r="51" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B51" s="93" t="s">
+      <c r="B51" s="97" t="s">
         <v>196</v>
       </c>
-      <c r="C51" s="93"/>
-      <c r="D51" s="93"/>
-      <c r="E51" s="93"/>
-      <c r="F51" s="93"/>
-      <c r="G51" s="93"/>
+      <c r="C51" s="97"/>
+      <c r="D51" s="97"/>
+      <c r="E51" s="97"/>
+      <c r="F51" s="97"/>
+      <c r="G51" s="97"/>
     </row>
     <row r="52" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B52" s="29" t="s">
@@ -59813,14 +59813,14 @@
       </c>
     </row>
     <row r="73" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B73" s="91" t="s">
+      <c r="B73" s="95" t="s">
         <v>201</v>
       </c>
-      <c r="C73" s="91"/>
-      <c r="D73" s="91"/>
-      <c r="E73" s="91"/>
-      <c r="F73" s="91"/>
-      <c r="G73" s="91"/>
+      <c r="C73" s="95"/>
+      <c r="D73" s="95"/>
+      <c r="E73" s="95"/>
+      <c r="F73" s="95"/>
+      <c r="G73" s="95"/>
     </row>
     <row r="74" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B74" s="17" t="s">
@@ -59915,14 +59915,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="95" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
     </row>
     <row r="3" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
@@ -59985,14 +59985,14 @@
       </c>
     </row>
     <row r="22" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="95" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="95"/>
+      <c r="G22" s="95"/>
     </row>
     <row r="23" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="22" t="s">
@@ -60138,14 +60138,14 @@
       <c r="H29" s="20"/>
     </row>
     <row r="47" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B47" s="91" t="s">
+      <c r="B47" s="95" t="s">
         <v>150</v>
       </c>
-      <c r="C47" s="91"/>
-      <c r="D47" s="91"/>
-      <c r="E47" s="91"/>
-      <c r="F47" s="91"/>
-      <c r="G47" s="91"/>
+      <c r="C47" s="95"/>
+      <c r="D47" s="95"/>
+      <c r="E47" s="95"/>
+      <c r="F47" s="95"/>
+      <c r="G47" s="95"/>
     </row>
     <row r="48" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B48" s="21" t="s">
@@ -60268,14 +60268,14 @@
       </c>
     </row>
     <row r="71" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B71" s="95" t="s">
+      <c r="B71" s="99" t="s">
         <v>157</v>
       </c>
-      <c r="C71" s="95"/>
-      <c r="D71" s="95"/>
-      <c r="E71" s="95"/>
-      <c r="F71" s="95"/>
-      <c r="G71" s="95"/>
+      <c r="C71" s="99"/>
+      <c r="D71" s="99"/>
+      <c r="E71" s="99"/>
+      <c r="F71" s="99"/>
+      <c r="G71" s="99"/>
     </row>
     <row r="72" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B72" s="17" t="s">
@@ -60338,14 +60338,14 @@
       </c>
     </row>
     <row r="92" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B92" s="91" t="s">
+      <c r="B92" s="95" t="s">
         <v>164</v>
       </c>
-      <c r="C92" s="91"/>
-      <c r="D92" s="91"/>
-      <c r="E92" s="91"/>
-      <c r="F92" s="91"/>
-      <c r="G92" s="91"/>
+      <c r="C92" s="95"/>
+      <c r="D92" s="95"/>
+      <c r="E92" s="95"/>
+      <c r="F92" s="95"/>
+      <c r="G92" s="95"/>
     </row>
     <row r="93" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B93" s="17" t="s">
@@ -60408,14 +60408,14 @@
       </c>
     </row>
     <row r="113" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B113" s="91" t="s">
+      <c r="B113" s="95" t="s">
         <v>172</v>
       </c>
-      <c r="C113" s="92"/>
-      <c r="D113" s="92"/>
-      <c r="E113" s="92"/>
-      <c r="F113" s="92"/>
-      <c r="G113" s="92"/>
+      <c r="C113" s="96"/>
+      <c r="D113" s="96"/>
+      <c r="E113" s="96"/>
+      <c r="F113" s="96"/>
+      <c r="G113" s="96"/>
     </row>
     <row r="114" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B114" s="17" t="s">
@@ -60530,7 +60530,7 @@
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D137">
         <f>(C115+C116)/SUM(C115:C118)</f>
@@ -60601,12 +60601,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B1" s="96" t="s">
-        <v>266</v>
-      </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
+      <c r="B1" s="100" t="s">
+        <v>264</v>
+      </c>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
     </row>
     <row r="2" spans="2:18" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -60621,15 +60621,15 @@
       <c r="E2" t="s">
         <v>206</v>
       </c>
-      <c r="M2" s="96" t="s">
+      <c r="M2" s="100" t="s">
         <v>215</v>
       </c>
-      <c r="N2" s="96"/>
-      <c r="P2" s="99" t="s">
+      <c r="N2" s="100"/>
+      <c r="P2" s="103" t="s">
         <v>214</v>
       </c>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="101"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="105"/>
     </row>
     <row r="3" spans="2:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -61044,10 +61044,10 @@
       <c r="L12" s="34"/>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
-      <c r="P12" s="102" t="s">
+      <c r="P12" s="106" t="s">
         <v>220</v>
       </c>
-      <c r="Q12" s="102"/>
+      <c r="Q12" s="106"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
@@ -61085,8 +61085,8 @@
         <f>GETPIVOTDATA("count",$G$3,"feature","hypertension","stroke_status","no stroke")*GETPIVOTDATA("count",$G$3,"feature","hypertension","category","hypertension")/GETPIVOTDATA("count",$G$3,"feature","hypertension")</f>
         <v>262.09113179813818</v>
       </c>
-      <c r="P13" s="102"/>
-      <c r="Q13" s="102"/>
+      <c r="P13" s="106"/>
+      <c r="Q13" s="106"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -61124,8 +61124,8 @@
         <f>GETPIVOTDATA("count",$G$3,"feature","hypertension","stroke_status","no stroke")*GETPIVOTDATA("count",$G$3,"feature","hypertension","category","no hypertension")/GETPIVOTDATA("count",$G$3,"feature","hypertension")</f>
         <v>3729.9088682018619</v>
       </c>
-      <c r="P14" s="102"/>
-      <c r="Q14" s="102"/>
+      <c r="P14" s="106"/>
+      <c r="Q14" s="106"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
@@ -61155,8 +61155,8 @@
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
-      <c r="P15" s="102"/>
-      <c r="Q15" s="102"/>
+      <c r="P15" s="106"/>
+      <c r="Q15" s="106"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -61194,8 +61194,8 @@
         <f>GETPIVOTDATA("count",$G$3,"feature","residence_type","stroke_status","no stroke")*GETPIVOTDATA("count",$G$3,"feature","residence_type","category","rural")/GETPIVOTDATA("count",$G$3,"feature","residence_type")</f>
         <v>1981.3307202351789</v>
       </c>
-      <c r="P16" s="102"/>
-      <c r="Q16" s="102"/>
+      <c r="P16" s="106"/>
+      <c r="Q16" s="106"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
@@ -61233,8 +61233,8 @@
         <f>GETPIVOTDATA("count",$G$3,"feature","residence_type","stroke_status","no stroke")*GETPIVOTDATA("count",$G$3,"feature","residence_type","category","urban")/GETPIVOTDATA("count",$G$3,"feature","residence_type")</f>
         <v>2010.6692797648211</v>
       </c>
-      <c r="P17" s="102"/>
-      <c r="Q17" s="102"/>
+      <c r="P17" s="106"/>
+      <c r="Q17" s="106"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
@@ -61264,8 +61264,8 @@
       <c r="L18" s="34"/>
       <c r="M18" s="34"/>
       <c r="N18" s="34"/>
-      <c r="P18" s="102"/>
-      <c r="Q18" s="102"/>
+      <c r="P18" s="106"/>
+      <c r="Q18" s="106"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -61303,8 +61303,8 @@
         <f>GETPIVOTDATA("count",$G$3,"feature","smoking_status","stroke_status","no stroke")*GETPIVOTDATA("count",$G$3,"feature","smoking_status","category","formerly smoked")/GETPIVOTDATA("count",$G$3,"feature","smoking_status")</f>
         <v>572.10191082802544</v>
       </c>
-      <c r="P19" s="102"/>
-      <c r="Q19" s="102"/>
+      <c r="P19" s="106"/>
+      <c r="Q19" s="106"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
@@ -61379,10 +61379,10 @@
         <f>GETPIVOTDATA("count",$G$3,"feature","smoking_status","stroke_status","no stroke")*GETPIVOTDATA("count",$G$3,"feature","smoking_status","category","smokes")/GETPIVOTDATA("count",$G$3,"feature","smoking_status")</f>
         <v>644.47035766780994</v>
       </c>
-      <c r="P21" s="98" t="s">
+      <c r="P21" s="102" t="s">
         <v>218</v>
       </c>
-      <c r="Q21" s="98"/>
+      <c r="Q21" s="102"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
@@ -61578,11 +61578,11 @@
         <f>GETPIVOTDATA("count",$G$3,"feature","work_type","stroke_status","no stroke")*GETPIVOTDATA("count",$G$3,"feature","work_type","category","never_worked")/GETPIVOTDATA("count",$G$3,"feature","work_type")</f>
         <v>21.514943655071043</v>
       </c>
-      <c r="P26" s="97" t="s">
+      <c r="P26" s="101" t="s">
         <v>219</v>
       </c>
-      <c r="Q26" s="97"/>
-      <c r="R26" s="97"/>
+      <c r="Q26" s="101"/>
+      <c r="R26" s="101"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
@@ -61620,9 +61620,9 @@
         <f>GETPIVOTDATA("count",$G$3,"feature","work_type","stroke_status","no stroke")*GETPIVOTDATA("count",$G$3,"feature","work_type","category","private")/GETPIVOTDATA("count",$G$3,"feature","work_type")</f>
         <v>2356.8642822146007</v>
       </c>
-      <c r="P27" s="97"/>
-      <c r="Q27" s="97"/>
-      <c r="R27" s="97"/>
+      <c r="P27" s="101"/>
+      <c r="Q27" s="101"/>
+      <c r="R27" s="101"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
@@ -61657,9 +61657,9 @@
         <f>GETPIVOTDATA("count",$G$3,"feature","work_type","stroke_status","no stroke")*GETPIVOTDATA("count",$G$3,"feature","work_type","category","self-employed")/GETPIVOTDATA("count",$G$3,"feature","work_type")</f>
         <v>427.36501714845662</v>
       </c>
-      <c r="P28" s="97"/>
-      <c r="Q28" s="97"/>
-      <c r="R28" s="97"/>
+      <c r="P28" s="101"/>
+      <c r="Q28" s="101"/>
+      <c r="R28" s="101"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
@@ -61686,9 +61686,9 @@
       <c r="J29">
         <v>2410</v>
       </c>
-      <c r="P29" s="97"/>
-      <c r="Q29" s="97"/>
-      <c r="R29" s="97"/>
+      <c r="P29" s="101"/>
+      <c r="Q29" s="101"/>
+      <c r="R29" s="101"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
@@ -61715,9 +61715,9 @@
       <c r="J30">
         <v>437</v>
       </c>
-      <c r="P30" s="97"/>
-      <c r="Q30" s="97"/>
-      <c r="R30" s="97"/>
+      <c r="P30" s="101"/>
+      <c r="Q30" s="101"/>
+      <c r="R30" s="101"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
@@ -61744,9 +61744,9 @@
       <c r="J31">
         <v>28574</v>
       </c>
-      <c r="P31" s="97"/>
-      <c r="Q31" s="97"/>
-      <c r="R31" s="97"/>
+      <c r="P31" s="101"/>
+      <c r="Q31" s="101"/>
+      <c r="R31" s="101"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
@@ -61761,9 +61761,9 @@
       <c r="E32">
         <v>685</v>
       </c>
-      <c r="P32" s="97"/>
-      <c r="Q32" s="97"/>
-      <c r="R32" s="97"/>
+      <c r="P32" s="101"/>
+      <c r="Q32" s="101"/>
+      <c r="R32" s="101"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
@@ -61778,9 +61778,9 @@
       <c r="E33">
         <v>16</v>
       </c>
-      <c r="P33" s="97"/>
-      <c r="Q33" s="97"/>
-      <c r="R33" s="97"/>
+      <c r="P33" s="101"/>
+      <c r="Q33" s="101"/>
+      <c r="R33" s="101"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
@@ -61795,9 +61795,9 @@
       <c r="E34">
         <v>510</v>
       </c>
-      <c r="P34" s="97"/>
-      <c r="Q34" s="97"/>
-      <c r="R34" s="97"/>
+      <c r="P34" s="101"/>
+      <c r="Q34" s="101"/>
+      <c r="R34" s="101"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
@@ -61812,9 +61812,9 @@
       <c r="E35">
         <v>22</v>
       </c>
-      <c r="P35" s="97"/>
-      <c r="Q35" s="97"/>
-      <c r="R35" s="97"/>
+      <c r="P35" s="101"/>
+      <c r="Q35" s="101"/>
+      <c r="R35" s="101"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B36" t="s">

</xml_diff>